<commit_message>
Fix record, changed "Ritwik" to "Jerald"
</commit_message>
<xml_diff>
--- a/Avalon_Ianthe.xlsx
+++ b/Avalon_Ianthe.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/A19Sean/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/A19Sean/Documents/project-arthur/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B927ACA-DEF9-AC4A-A656-7F597424D2AA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B77BEA-5652-0242-BFCE-188E8710C4EA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="2" xr2:uid="{33E7807F-E86D-6543-BBBD-F58C2CA9F7BF}"/>
   </bookViews>
@@ -943,7 +943,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1044,7 +1044,7 @@
         <v>43327</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>

</xml_diff>